<commit_message>
generador de certificado de propiedad intelectual
</commit_message>
<xml_diff>
--- a/dist/database.xlsx
+++ b/dist/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e93e8a63036fd941/Documentos/PROYECTOS/SOFTWARE PELUQUERIA/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_FBC55805C57F3883062E954A6A14D4AE722EC2D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA853BBE-5422-495B-BCF5-EC45A304BE71}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3E3DD4549AEA6240BE44F136EDB2F222732E845E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C6C97AB-192A-474D-9E94-072854FD546B}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="390" windowWidth="19290" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="-120" windowWidth="19530" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicios" sheetId="1" r:id="rId1"/>
@@ -1892,7 +1892,7 @@
   <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>